<commit_message>
Thêm một số comment
</commit_message>
<xml_diff>
--- a/Phân chia công việc.xlsx
+++ b/Phân chia công việc.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Huynh\Downloads\Baitap_Capstone_Nhom1-master (18)\Baitap_Capstone_Nhom1-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Baitap_Capstone_Nhom11\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
   <si>
     <t>Tasks Name</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Quỳnh không có nhu cầu làm bài tập</t>
+  </si>
+  <si>
+    <t>sort và filter</t>
   </si>
 </sst>
 </file>
@@ -252,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -292,6 +295,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -510,10 +514,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -735,6 +739,36 @@
       </c>
       <c r="J7" s="11"/>
     </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="8">
+        <v>45244</v>
+      </c>
+      <c r="C8" s="8">
+        <v>45244</v>
+      </c>
+      <c r="D8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F8" s="8">
+        <v>45244</v>
+      </c>
+      <c r="G8" s="8">
+        <v>45244</v>
+      </c>
+      <c r="H8" s="9">
+        <v>2</v>
+      </c>
+      <c r="I8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="15"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J2:J3"/>

</xml_diff>